<commit_message>
Updated some values, notes and the training process.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\gpu_tu_dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DE3020-B8C7-47B9-8FC8-40E3FB49BD65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8C4D2D-2632-4E02-84BA-43692C9868C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="0" windowWidth="21405" windowHeight="15435" firstSheet="2" activeTab="2" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="2235" yWindow="-270" windowWidth="21405" windowHeight="15435" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
-    <sheet name="TF2TF_ML_ENG" sheetId="1" r:id="rId1"/>
-    <sheet name="TF2TF_ML_DE_MIX" sheetId="5" r:id="rId2"/>
-    <sheet name="TF2TF_DE_DE_MIX" sheetId="8" r:id="rId3"/>
+    <sheet name="BERT2BERT_ML_ENG_MIX" sheetId="1" r:id="rId1"/>
+    <sheet name="BERT2BERT_ML_DE_MIX" sheetId="5" r:id="rId2"/>
+    <sheet name="BERT2BERT_DE_DE_MIX" sheetId="8" r:id="rId3"/>
+    <sheet name="XLMR2XLMR_ML_DE_MIX" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
   <si>
     <t>Language</t>
   </si>
@@ -90,6 +91,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>RoBERTa (multilingual, cased)</t>
   </si>
 </sst>
 </file>
@@ -212,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -252,15 +256,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -378,7 +373,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_ML_ENG!$C$2</c:f>
+              <c:f>BERT2BERT_ML_ENG_MIX!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -413,10 +408,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_ML_ENG!$C$3:$C$20</c:f>
+              <c:f>BERT2BERT_ML_ENG_MIX!$C$3:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>4.2798999999999996</c:v>
                 </c:pt>
@@ -470,6 +465,30 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>2.222</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.1145</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1008</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.0874000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0870000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0815999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.0752000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.0634000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.0613999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,7 +754,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_ML_ENG!$D$2</c:f>
+              <c:f>BERT2BERT_ML_ENG_MIX!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -758,10 +777,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_ML_ENG!$D$3:$D$20</c:f>
+              <c:f>BERT2BERT_ML_ENG_MIX!$D$3:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>3.1E-2</c:v>
                 </c:pt>
@@ -815,6 +834,30 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.10970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1074</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.10970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.10970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.1084</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.10879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.11070000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.11169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10979999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -831,7 +874,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_ML_ENG!$E$2</c:f>
+              <c:f>BERT2BERT_ML_ENG_MIX!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -854,10 +897,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_ML_ENG!$E$3:$E$20</c:f>
+              <c:f>BERT2BERT_ML_ENG_MIX!$E$3:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>4.41E-2</c:v>
                 </c:pt>
@@ -911,6 +954,30 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.15859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1598</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.16489999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.16239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.1638</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1641</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.1643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -927,7 +994,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_ML_ENG!$F$2</c:f>
+              <c:f>BERT2BERT_ML_ENG_MIX!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -950,10 +1017,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_ML_ENG!$F$3:$F$20</c:f>
+              <c:f>BERT2BERT_ML_ENG_MIX!$F$3:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>3.4700000000000002E-2</c:v>
                 </c:pt>
@@ -1007,6 +1074,30 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.12570000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1245</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12659999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.12740000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.12590000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.12690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.128</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.12859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.1273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1274,7 +1365,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_ML_DE_MIX!$C$2</c:f>
+              <c:f>BERT2BERT_ML_DE_MIX!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1309,7 +1400,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_ML_DE_MIX!$C$3:$C$10</c:f>
+              <c:f>BERT2BERT_ML_DE_MIX!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1601,7 +1692,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_ML_DE_MIX!$D$2</c:f>
+              <c:f>BERT2BERT_ML_DE_MIX!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1624,7 +1715,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_ML_DE_MIX!$D$3:$D$10</c:f>
+              <c:f>BERT2BERT_ML_DE_MIX!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1667,7 +1758,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_ML_DE_MIX!$E$2</c:f>
+              <c:f>BERT2BERT_ML_DE_MIX!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1690,7 +1781,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_ML_DE_MIX!$E$3:$E$10</c:f>
+              <c:f>BERT2BERT_ML_DE_MIX!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1733,7 +1824,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_ML_DE_MIX!$F$2</c:f>
+              <c:f>BERT2BERT_ML_DE_MIX!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1756,7 +1847,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_ML_DE_MIX!$F$3:$F$10</c:f>
+              <c:f>BERT2BERT_ML_DE_MIX!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2050,7 +2141,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_DE_DE_MIX!$C$2</c:f>
+              <c:f>BERT2BERT_DE_DE_MIX!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2073,7 +2164,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_DE_DE_MIX!$C$3:$C$10</c:f>
+              <c:f>BERT2BERT_DE_DE_MIX!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2364,7 +2455,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_DE_DE_MIX!$D$2</c:f>
+              <c:f>BERT2BERT_DE_DE_MIX!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2387,7 +2478,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_DE_DE_MIX!$D$3:$D$10</c:f>
+              <c:f>BERT2BERT_DE_DE_MIX!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2430,7 +2521,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_DE_DE_MIX!$E$2</c:f>
+              <c:f>BERT2BERT_DE_DE_MIX!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2453,7 +2544,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_DE_DE_MIX!$E$3:$E$10</c:f>
+              <c:f>BERT2BERT_DE_DE_MIX!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2496,7 +2587,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>TF2TF_DE_DE_MIX!$F$2</c:f>
+              <c:f>BERT2BERT_DE_DE_MIX!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2519,7 +2610,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>TF2TF_DE_DE_MIX!$F$3:$F$10</c:f>
+              <c:f>BERT2BERT_DE_DE_MIX!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2554,6 +2645,673 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-05A0-4C05-B288-3A7E4C7ED1BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="533795144"/>
+        <c:axId val="533794816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="533795144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533794816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="533794816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533795144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="21835E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5CE7-4141-A035-A9CBE77FA7C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="530566160"/>
+        <c:axId val="530567800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="530566160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530567800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="530567800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530566160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" b="1">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Scores</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Precision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="21835E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$D$3:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC6C-4F06-B8F7-0B691D7044BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="325D72"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EC6C-4F06-B8F7-0B691D7044BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Measure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="A74343"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EC6C-4F06-B8F7-0B691D7044BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2998,6 +3756,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5540,6 +6378,1025 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6296,6 +8153,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7F77FDF-E816-410E-92D0-F8E30630D029}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6A0BF62-C523-4255-8A98-183E471745DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -6595,14 +8533,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7255D-F7D4-49BE-B381-76409DC043B4}">
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6622,10 +8560,10 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="19"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -6981,68 +8919,168 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="B21" s="6">
+        <v>2.12</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2.1145</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.1074</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.1598</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0.1245</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>2.23</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2.1008</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.10970000000000001</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.12659999999999999</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>2.34</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2.0874000000000001</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.10970000000000001</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.16489999999999999</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0.12740000000000001</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2.0870000000000002</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0.1084</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0.12590000000000001</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>2.56</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2.0815999999999999</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.10879999999999999</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.16389999999999999</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0.12690000000000001</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>2.67</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2.0752000000000002</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.1638</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0.128</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>2.79</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2.0634000000000001</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.11169999999999999</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.1641</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="C28" s="8">
+        <v>2.0613999999999999</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.10979999999999999</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.1643</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0.1273</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B29" s="17">
         <v>3</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="17">
-        <v>0.1023</v>
-      </c>
-      <c r="E21" s="14">
-        <v>0.15010000000000001</v>
-      </c>
-      <c r="F21" s="18">
-        <v>0.1187</v>
-      </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="14">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0.1578</v>
+      </c>
+      <c r="F29" s="14">
+        <v>0.1211</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -7106,7 +9144,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7126,10 +9164,10 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="19"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -7308,7 +9346,7 @@
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="17">
         <v>3</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -7483,14 +9521,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E688F7-C154-410D-8981-819F715851A0}">
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7510,10 +9548,10 @@
       <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="19"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -7692,21 +9730,300 @@
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="17">
         <v>3</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="18">
         <v>0.14649999999999999</v>
       </c>
       <c r="E11" s="14">
         <v>0.24199999999999999</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="18">
         <v>0.16850000000000001</v>
       </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42CEBC-4DF1-4EAE-9662-1F6C023E63EA}">
+  <dimension ref="A2:I34"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="9"/>
+      <c r="H3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added some more notes.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\gpu_tu_dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8C4D2D-2632-4E02-84BA-43692C9868C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5069835C-FCD9-4766-930B-FB69814C3943}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="-270" windowWidth="21405" windowHeight="15435" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="2235" yWindow="-270" windowWidth="21405" windowHeight="15435" firstSheet="1" activeTab="3" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT2BERT_ML_ENG_MIX" sheetId="1" r:id="rId1"/>
@@ -8533,7 +8533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7255D-F7D4-49BE-B381-76409DC043B4}">
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -9890,8 +9890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42CEBC-4DF1-4EAE-9662-1F6C023E63EA}">
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Created another presentation, continued training.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\gpu_tu_dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5069835C-FCD9-4766-930B-FB69814C3943}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA73FAF-5602-4C53-82A9-5AAF7123A332}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="-270" windowWidth="21405" windowHeight="15435" firstSheet="1" activeTab="3" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT2BERT_ML_ENG_MIX" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
     <t>-</t>
   </si>
   <si>
-    <t>RoBERTa (multilingual, cased)</t>
+    <t>XLM-RoBERTa (multilingual, cased)</t>
   </si>
 </sst>
 </file>
@@ -257,13 +257,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8560,10 +8560,10 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -9066,7 +9066,7 @@
       <c r="A29" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="16">
         <v>3</v>
       </c>
       <c r="C29" s="14" t="s">
@@ -9164,10 +9164,10 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -9346,7 +9346,7 @@
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>3</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -9548,10 +9548,10 @@
       <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -9730,19 +9730,19 @@
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>3</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>0.14649999999999999</v>
       </c>
       <c r="E11" s="14">
         <v>0.24199999999999999</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>0.16850000000000001</v>
       </c>
       <c r="G11" s="1"/>
@@ -9891,7 +9891,7 @@
   <dimension ref="A2:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9917,10 +9917,10 @@
       <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
@@ -10019,11 +10019,11 @@
       <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="18"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Did more training with RoBERTa.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\gpu_tu_dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA73FAF-5602-4C53-82A9-5AAF7123A332}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624D50E0-DD5E-4C06-9FD7-D6B93106B53B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT2BERT_ML_ENG_MIX" sheetId="1" r:id="rId1"/>
     <sheet name="BERT2BERT_ML_DE_MIX" sheetId="5" r:id="rId2"/>
     <sheet name="BERT2BERT_DE_DE_MIX" sheetId="8" r:id="rId3"/>
     <sheet name="XLMR2XLMR_ML_DE_MIX" sheetId="9" r:id="rId4"/>
+    <sheet name="COMPARISON" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="35">
   <si>
     <t>Language</t>
   </si>
@@ -66,9 +67,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>BERT (multilingual, cased)</t>
-  </si>
-  <si>
     <t>Metadata</t>
   </si>
   <si>
@@ -93,7 +91,71 @@
     <t>-</t>
   </si>
   <si>
-    <t>XLM-RoBERTa (multilingual, cased)</t>
+    <t>BERT-BASE-MULTILINGUAL-CASED</t>
+  </si>
+  <si>
+    <t>XLM-ROBERTA-LARGE</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>GERMAN</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>BERT-BASE-GERMAN-CASED</t>
+  </si>
+  <si>
+    <t>CARDIFFNLP/TWITTER-XLM-ROBERTA-BASE</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>TRAIN_
+CORPUS_
+WIKI</t>
+  </si>
+  <si>
+    <t>TRAIN_
+CORPUS_
+NEWS</t>
+  </si>
+  <si>
+    <t>TEST_
+CORPUS_
+WIKI</t>
+  </si>
+  <si>
+    <t>TEST_
+CORPUS_
+NEWS</t>
+  </si>
+  <si>
+    <t>ROUGE_
+PRECISION</t>
+  </si>
+  <si>
+    <t>ROUGE_
+RECALL</t>
+  </si>
+  <si>
+    <t>ROUGE_
+MEASURE</t>
+  </si>
+  <si>
+    <t>ENCODER/ 
+DECODER/
+TOKENIZER</t>
   </si>
 </sst>
 </file>
@@ -135,7 +197,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +207,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF325D72"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -216,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -266,6 +334,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -274,9 +359,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF325D72"/>
       <color rgb="FFA74343"/>
       <color rgb="FF21835E"/>
-      <color rgb="FF325D72"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2927,10 +3012,121 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$C$3:$C$10</c:f>
+              <c:f>XLMR2XLMR_ML_DE_MIX!$C$3:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>8.1145999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8155999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5437000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0956000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.6414</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6403999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1712999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8631000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6537999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4325999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.2911000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.1345000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0064000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.9178999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8612000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.7999000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.7490999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.7258</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.6625999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.6406000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.5825</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5712999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5459000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.5154999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.4079999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.3584000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.3721999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.3546</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.3736999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.3241000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.3178000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.3041999999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.2854999999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.2852999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.2669000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.2715999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3215,12 +3411,65 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$D$3:$D$10</c:f>
+              <c:f>(XLMR2XLMR_ML_DE_MIX!$D$7,XLMR2XLMR_ML_DE_MIX!$D$12,XLMR2XLMR_ML_DE_MIX!$D$17,XLMR2XLMR_ML_DE_MIX!$D$22,XLMR2XLMR_ML_DE_MIX!$D$27,XLMR2XLMR_ML_DE_MIX!$D$32,XLMR2XLMR_ML_DE_MIX!$D$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.6399999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12920000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15079999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1525</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1583</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3257,19 +3506,77 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B9B8-4352-B83D-6F7A5C87D675}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$E$3:$E$10</c:f>
+              <c:f>(XLMR2XLMR_ML_DE_MIX!$E$7,XLMR2XLMR_ML_DE_MIX!$E$12,XLMR2XLMR_ML_DE_MIX!$E$17,XLMR2XLMR_ML_DE_MIX!$E$22,XLMR2XLMR_ML_DE_MIX!$E$27,XLMR2XLMR_ML_DE_MIX!$E$32,XLMR2XLMR_ML_DE_MIX!$E$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.2400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1842</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2243</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26889999999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EC6C-4F06-B8F7-0B691D7044BE}"/>
+              <c16:uniqueId val="{00000005-B9B8-4352-B83D-6F7A5C87D675}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3299,19 +3606,72 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$F$3:$F$10</c:f>
+              <c:f>(XLMR2XLMR_ML_DE_MIX!$F$7,XLMR2XLMR_ML_DE_MIX!$F$12,XLMR2XLMR_ML_DE_MIX!$F$17,XLMR2XLMR_ML_DE_MIX!$F$22,XLMR2XLMR_ML_DE_MIX!$F$27,XLMR2XLMR_ML_DE_MIX!$F$32,XLMR2XLMR_ML_DE_MIX!$F$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.4399999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1179</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1515</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1845</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-EC6C-4F06-B8F7-0B691D7044BE}"/>
+              <c16:uniqueId val="{00000006-B9B8-4352-B83D-6F7A5C87D675}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3334,6 +3694,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8534,7 +8895,7 @@
   <dimension ref="A2:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8561,7 +8922,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="18"/>
     </row>
@@ -8609,7 +8970,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -8633,7 +8994,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -8654,10 +9015,10 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -8678,10 +9039,10 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -9064,13 +9425,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" s="16">
         <v>3</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D29" s="14">
         <v>0.10249999999999999</v>
@@ -9165,7 +9526,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="18"/>
     </row>
@@ -9189,7 +9550,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -9213,7 +9574,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -9237,7 +9598,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -9258,10 +9619,10 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -9282,10 +9643,10 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -9344,13 +9705,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="16">
         <v>3</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="14">
         <v>0.15049999999999999</v>
@@ -9549,7 +9910,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="18"/>
     </row>
@@ -9573,7 +9934,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -9597,7 +9958,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -9621,7 +9982,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -9642,10 +10003,10 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -9666,10 +10027,10 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -9728,13 +10089,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="16">
         <v>3</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="17">
         <v>0.14649999999999999</v>
@@ -9888,9 +10249,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42CEBC-4DF1-4EAE-9662-1F6C023E63EA}">
-  <dimension ref="A2:I34"/>
+  <dimension ref="A2:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -9918,13 +10279,17 @@
         <v>7</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="C3" s="7">
+        <v>8.1145999999999994</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="3"/>
       <c r="F3" s="9"/>
@@ -9932,12 +10297,16 @@
         <v>0</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="C4" s="8">
+        <v>6.8155999999999999</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="3"/>
       <c r="F4" s="10"/>
@@ -9950,8 +10319,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="C5" s="8">
+        <v>6.5437000000000003</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="3"/>
       <c r="F5" s="10"/>
@@ -9964,196 +10337,484 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="C6" s="8">
+        <v>6.0956000000000001</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="3"/>
       <c r="F6" s="10"/>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="10"/>
+      <c r="B7" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>5.6414</v>
+      </c>
+      <c r="D7" s="8">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5.4399999999999997E-2</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="C8" s="8">
+        <v>5.1859999999999999</v>
+      </c>
       <c r="D8" s="8"/>
       <c r="E8" s="3"/>
       <c r="F8" s="10"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4.6403999999999996</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="3"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="6">
+        <v>0.63</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4.1712999999999996</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="3"/>
       <c r="F10" s="10"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="17"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="6">
+        <v>0.71</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3.8631000000000002</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="B12" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="C12" s="8">
+        <v>3.6537999999999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.1842</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.1179</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="C13" s="8">
+        <v>3.4325999999999999</v>
+      </c>
+      <c r="D13" s="8"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="C14" s="8">
+        <v>3.2911000000000001</v>
+      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="6">
+        <v>1.03</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3.1345000000000001</v>
+      </c>
+      <c r="D15" s="8"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3.0064000000000002</v>
+      </c>
+      <c r="D16" s="8"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>1.19</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2.9178999999999999</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.12920000000000001</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.2243</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.1515</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2.8612000000000002</v>
+      </c>
+      <c r="D18" s="8"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>1.34</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2.7999000000000001</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>1.42</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2.7490999999999999</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="10"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2.7258</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>1.58</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2.6625999999999999</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.16400000000000001</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>1.66</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2.6406000000000001</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>1.74</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2.5825</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>1.82</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2.5712999999999999</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="10"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2.5459000000000001</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="10"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>1.98</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2.5154999999999998</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.15079999999999999</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.17599999999999999</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>2.06</v>
+      </c>
+      <c r="C28" s="8">
+        <v>2.4079999999999999</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>2.14</v>
+      </c>
+      <c r="C29" s="8">
+        <v>2.3584000000000001</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="10"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <v>2.21</v>
+      </c>
+      <c r="C30" s="8">
+        <v>2.3721999999999999</v>
+      </c>
+      <c r="D30" s="8"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="F30" s="10"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>2.29</v>
+      </c>
+      <c r="C31" s="8">
+        <v>2.3546</v>
+      </c>
+      <c r="D31" s="8"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="F31" s="10"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="6">
+        <v>2.37</v>
+      </c>
+      <c r="C32" s="8">
+        <v>2.3736999999999999</v>
+      </c>
+      <c r="D32" s="8">
+        <v>0.1525</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0.1789</v>
+      </c>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C33" s="8">
+        <v>2.3241000000000001</v>
+      </c>
+      <c r="D33" s="8"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="F33" s="10"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="C34" s="8">
+        <v>2.3178000000000001</v>
+      </c>
+      <c r="D34" s="8"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="10"/>
       <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <v>2.61</v>
+      </c>
+      <c r="C35" s="8">
+        <v>2.3041999999999998</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="6">
+        <v>2.69</v>
+      </c>
+      <c r="C36" s="8">
+        <v>2.2854999999999999</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <v>2.77</v>
+      </c>
+      <c r="C37" s="8">
+        <v>2.2852999999999999</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0.1583</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.26889999999999997</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.1845</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
+        <v>2.85</v>
+      </c>
+      <c r="C38" s="8">
+        <v>2.2669000000000001</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
+        <v>2.93</v>
+      </c>
+      <c r="C39" s="8">
+        <v>2.2715999999999998</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="16">
+        <v>3</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="17">
+        <v>0.13950000000000001</v>
+      </c>
+      <c r="E40" s="14">
+        <v>0.23019999999999999</v>
+      </c>
+      <c r="F40" s="17">
+        <v>0.16089999999999999</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10163,4 +10824,395 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F46F1A2-3464-46AB-AC0B-0CBD57F6E68E}">
+  <dimension ref="A2:J29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="7" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="19">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="I3" s="19">
+        <v>0.1578</v>
+      </c>
+      <c r="J3" s="24">
+        <v>0.1211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="19">
+        <v>0.15049999999999999</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0.24560000000000001</v>
+      </c>
+      <c r="J4" s="25">
+        <v>0.17249999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="19">
+        <v>0.14649999999999999</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="J5" s="25">
+        <v>0.16850000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0.13950000000000001</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.23019999999999999</v>
+      </c>
+      <c r="J6" s="25">
+        <v>0.16089999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="23"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="23"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Continued training as always.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\gpu_tu_dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624D50E0-DD5E-4C06-9FD7-D6B93106B53B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC05907-453A-4557-950F-51597294953A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="7395" yWindow="165" windowWidth="21405" windowHeight="15435" activeTab="4" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
-    <sheet name="BERT2BERT_ML_ENG_MIX" sheetId="1" r:id="rId1"/>
-    <sheet name="BERT2BERT_ML_DE_MIX" sheetId="5" r:id="rId2"/>
-    <sheet name="BERT2BERT_DE_DE_MIX" sheetId="8" r:id="rId3"/>
-    <sheet name="XLMR2XLMR_ML_DE_MIX" sheetId="9" r:id="rId4"/>
-    <sheet name="COMPARISON" sheetId="10" r:id="rId5"/>
+    <sheet name="BERT_ML_ENG_MIX" sheetId="1" r:id="rId1"/>
+    <sheet name="BERT_ML_DE_MIX" sheetId="5" r:id="rId2"/>
+    <sheet name="BERT_DE_DE_MIX" sheetId="8" r:id="rId3"/>
+    <sheet name="XLMR_ML_DE_MIX" sheetId="9" r:id="rId4"/>
+    <sheet name="GBERT_DE_DE_MIX" sheetId="11" r:id="rId5"/>
+    <sheet name="BERT_ML_DE_MIX_EXP" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="36">
   <si>
     <t>Language</t>
   </si>
@@ -121,41 +122,44 @@
     <t>0.1</t>
   </si>
   <si>
-    <t>TRAIN_
-CORPUS_
+    <t>ENCODER 
+DECODER
+TOKENIZER</t>
+  </si>
+  <si>
+    <t>TRAIN
+CORPUS
 WIKI</t>
   </si>
   <si>
-    <t>TRAIN_
-CORPUS_
+    <t>TRAIN
+CORPUS
 NEWS</t>
   </si>
   <si>
-    <t>TEST_
-CORPUS_
+    <t>TEST
+CORPUS
 WIKI</t>
   </si>
   <si>
-    <t>TEST_
-CORPUS_
+    <t>TEST
+CORPUS
 NEWS</t>
   </si>
   <si>
-    <t>ROUGE_
+    <t>ROUGE
 PRECISION</t>
   </si>
   <si>
-    <t>ROUGE_
+    <t>ROUGE
 RECALL</t>
   </si>
   <si>
-    <t>ROUGE_
+    <t>ROUGE
 MEASURE</t>
   </si>
   <si>
-    <t>ENCODER/ 
-DECODER/
-TOKENIZER</t>
+    <t>DEEPSET/GBERT-BASE</t>
   </si>
 </sst>
 </file>
@@ -284,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -325,6 +329,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -345,10 +352,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -458,7 +468,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_ML_ENG_MIX!$C$2</c:f>
+              <c:f>BERT_ML_ENG_MIX!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -493,7 +503,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_ML_ENG_MIX!$C$3:$C$28</c:f>
+              <c:f>BERT_ML_ENG_MIX!$C$3:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="26"/>
@@ -756,6 +766,420 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" b="1">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Scores</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GBERT_DE_DE_MIX!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Precision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="21835E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>GBERT_DE_DE_MIX!$D$3:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="4">
+                  <c:v>0.1147</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-31E4-420A-A52A-0261E3DCEBBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GBERT_DE_DE_MIX!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="325D72"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>GBERT_DE_DE_MIX!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="4">
+                  <c:v>0.21729999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-31E4-420A-A52A-0261E3DCEBBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GBERT_DE_DE_MIX!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Measure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="A74343"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>GBERT_DE_DE_MIX!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="4">
+                  <c:v>0.1389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-31E4-420A-A52A-0261E3DCEBBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="533795144"/>
+        <c:axId val="533794816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="533795144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533794816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="533794816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533795144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -839,7 +1263,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_ML_ENG_MIX!$D$2</c:f>
+              <c:f>BERT_ML_ENG_MIX!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -862,7 +1286,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_ML_ENG_MIX!$D$3:$D$28</c:f>
+              <c:f>BERT_ML_ENG_MIX!$D$3:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="26"/>
@@ -959,7 +1383,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_ML_ENG_MIX!$E$2</c:f>
+              <c:f>BERT_ML_ENG_MIX!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -982,7 +1406,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_ML_ENG_MIX!$E$3:$E$28</c:f>
+              <c:f>BERT_ML_ENG_MIX!$E$3:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1079,7 +1503,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_ML_ENG_MIX!$F$2</c:f>
+              <c:f>BERT_ML_ENG_MIX!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1102,7 +1526,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_ML_ENG_MIX!$F$3:$F$28</c:f>
+              <c:f>BERT_ML_ENG_MIX!$F$3:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1450,7 +1874,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_ML_DE_MIX!$C$2</c:f>
+              <c:f>BERT_ML_DE_MIX!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1485,7 +1909,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_ML_DE_MIX!$C$3:$C$10</c:f>
+              <c:f>BERT_ML_DE_MIX!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1777,7 +2201,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_ML_DE_MIX!$D$2</c:f>
+              <c:f>BERT_ML_DE_MIX!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1800,7 +2224,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_ML_DE_MIX!$D$3:$D$10</c:f>
+              <c:f>BERT_ML_DE_MIX!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1843,7 +2267,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_ML_DE_MIX!$E$2</c:f>
+              <c:f>BERT_ML_DE_MIX!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1866,7 +2290,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_ML_DE_MIX!$E$3:$E$10</c:f>
+              <c:f>BERT_ML_DE_MIX!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1909,7 +2333,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_ML_DE_MIX!$F$2</c:f>
+              <c:f>BERT_ML_DE_MIX!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1932,7 +2356,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_ML_DE_MIX!$F$3:$F$10</c:f>
+              <c:f>BERT_ML_DE_MIX!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2226,7 +2650,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_DE_DE_MIX!$C$2</c:f>
+              <c:f>BERT_DE_DE_MIX!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2249,7 +2673,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_DE_DE_MIX!$C$3:$C$10</c:f>
+              <c:f>BERT_DE_DE_MIX!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2540,7 +2964,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_DE_DE_MIX!$D$2</c:f>
+              <c:f>BERT_DE_DE_MIX!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2563,7 +2987,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_DE_DE_MIX!$D$3:$D$10</c:f>
+              <c:f>BERT_DE_DE_MIX!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2606,7 +3030,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_DE_DE_MIX!$E$2</c:f>
+              <c:f>BERT_DE_DE_MIX!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2629,7 +3053,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_DE_DE_MIX!$E$3:$E$10</c:f>
+              <c:f>BERT_DE_DE_MIX!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2672,7 +3096,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT2BERT_DE_DE_MIX!$F$2</c:f>
+              <c:f>BERT_DE_DE_MIX!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2695,7 +3119,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT2BERT_DE_DE_MIX!$F$3:$F$10</c:f>
+              <c:f>BERT_DE_DE_MIX!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2989,7 +3413,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$C$2</c:f>
+              <c:f>XLMR_ML_DE_MIX!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3012,7 +3436,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$C$3:$C$39</c:f>
+              <c:f>XLMR_ML_DE_MIX!$C$3:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="37"/>
@@ -3390,7 +3814,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$D$2</c:f>
+              <c:f>XLMR_ML_DE_MIX!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3445,7 +3869,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR2XLMR_ML_DE_MIX!$D$7,XLMR2XLMR_ML_DE_MIX!$D$12,XLMR2XLMR_ML_DE_MIX!$D$17,XLMR2XLMR_ML_DE_MIX!$D$22,XLMR2XLMR_ML_DE_MIX!$D$27,XLMR2XLMR_ML_DE_MIX!$D$32,XLMR2XLMR_ML_DE_MIX!$D$37)</c:f>
+              <c:f>(XLMR_ML_DE_MIX!$D$7,XLMR_ML_DE_MIX!$D$12,XLMR_ML_DE_MIX!$D$17,XLMR_ML_DE_MIX!$D$22,XLMR_ML_DE_MIX!$D$27,XLMR_ML_DE_MIX!$D$32,XLMR_ML_DE_MIX!$D$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3485,7 +3909,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$E$2</c:f>
+              <c:f>XLMR_ML_DE_MIX!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3545,7 +3969,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR2XLMR_ML_DE_MIX!$E$7,XLMR2XLMR_ML_DE_MIX!$E$12,XLMR2XLMR_ML_DE_MIX!$E$17,XLMR2XLMR_ML_DE_MIX!$E$22,XLMR2XLMR_ML_DE_MIX!$E$27,XLMR2XLMR_ML_DE_MIX!$E$32,XLMR2XLMR_ML_DE_MIX!$E$37)</c:f>
+              <c:f>(XLMR_ML_DE_MIX!$E$7,XLMR_ML_DE_MIX!$E$12,XLMR_ML_DE_MIX!$E$17,XLMR_ML_DE_MIX!$E$22,XLMR_ML_DE_MIX!$E$27,XLMR_ML_DE_MIX!$E$32,XLMR_ML_DE_MIX!$E$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3585,7 +4009,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>XLMR2XLMR_ML_DE_MIX!$F$2</c:f>
+              <c:f>XLMR_ML_DE_MIX!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3640,7 +4064,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR2XLMR_ML_DE_MIX!$F$7,XLMR2XLMR_ML_DE_MIX!$F$12,XLMR2XLMR_ML_DE_MIX!$F$17,XLMR2XLMR_ML_DE_MIX!$F$22,XLMR2XLMR_ML_DE_MIX!$F$27,XLMR2XLMR_ML_DE_MIX!$F$32,XLMR2XLMR_ML_DE_MIX!$F$37)</c:f>
+              <c:f>(XLMR_ML_DE_MIX!$F$7,XLMR_ML_DE_MIX!$F$12,XLMR_ML_DE_MIX!$F$17,XLMR_ML_DE_MIX!$F$22,XLMR_ML_DE_MIX!$F$27,XLMR_ML_DE_MIX!$F$32,XLMR_ML_DE_MIX!$F$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3877,7 +4301,333 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GBERT_DE_DE_MIX!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="21835E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>GBERT_DE_DE_MIX!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.9932999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5619000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1392000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8950999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7063000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5735000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4460999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2F0F-4A9D-9145-0FAFF4B4EDC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="530566160"/>
+        <c:axId val="530567800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="530566160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530567800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="530567800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530566160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4197,6 +4947,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4700,7 +5490,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5216,8 +6006,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5325,6 +6115,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5335,6 +6130,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5366,6 +6166,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5719,8 +6522,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5828,11 +6631,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5843,11 +6641,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5879,9 +6672,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6235,8 +7025,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6344,6 +7134,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -6354,6 +7149,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -6385,6 +7185,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6738,8 +7541,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6847,11 +7650,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -6862,11 +7660,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -6898,9 +7691,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7254,8 +8044,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7363,6 +8153,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -7373,6 +8168,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -7404,6 +8204,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7757,8 +8560,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7866,11 +8669,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -7881,11 +8679,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -7917,9 +8710,1025 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8595,6 +10404,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{894DCD04-5085-4646-94DA-95ED03FBE1BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E85E22-6818-4926-91BF-60564AB9F24A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -8921,10 +10811,10 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -9427,7 +11317,7 @@
       <c r="A29" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="17">
         <v>3</v>
       </c>
       <c r="C29" s="14" t="s">
@@ -9525,10 +11415,10 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -9707,7 +11597,7 @@
       <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="17">
         <v>3</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -9909,10 +11799,10 @@
       <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -10091,19 +11981,19 @@
       <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="17">
         <v>3</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="18">
         <v>0.14649999999999999</v>
       </c>
       <c r="E11" s="14">
         <v>0.24199999999999999</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="18">
         <v>0.16850000000000001</v>
       </c>
       <c r="G11" s="1"/>
@@ -10278,10 +12168,10 @@
       <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -10800,19 +12690,19 @@
       <c r="A40" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="17">
         <v>3</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="18">
         <v>0.13950000000000001</v>
       </c>
       <c r="E40" s="14">
         <v>0.23019999999999999</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F40" s="18">
         <v>0.16089999999999999</v>
       </c>
     </row>
@@ -10827,389 +12717,941 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AF756F-671F-47D9-8966-F6A5F7632BF1}">
+  <dimension ref="A2:I38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="C3" s="7">
+        <v>4.9932999999999996</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="9"/>
+      <c r="H3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.5619000000000001</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3.1392000000000002</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2.8950999999999998</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2.7063000000000001</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.1147</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.21729999999999999</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.1389</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2.5735000000000001</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2.4630000000000001</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2.4460999999999999</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2.3677000000000001</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>0.84</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2.2925</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.14280000000000001</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.25919999999999999</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.1709</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2.2827999999999999</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2.2237</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2.0314000000000001</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>1.17</v>
+      </c>
+      <c r="C16" s="8">
+        <v>2.0356000000000001</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>1.26</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2.0244</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.15490000000000001</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.27410000000000001</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.18379999999999999</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>1.34</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2.0076999999999998</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>1.42</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1.9990000000000001</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>1.51</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2.0032999999999999</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>1.59</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1.9758</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>1.67</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1.9495</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.161</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.28110000000000002</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.19009999999999999</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>1.76</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1.9435</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>1.84</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1.9577</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>1.93</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1.9008</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>2.09</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1.7516</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.28339999999999999</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.19220000000000001</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1.7401</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1.7418</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <v>2.34</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1.7321</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1.7477</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1.7448999999999999</v>
+      </c>
+      <c r="D32" s="8">
+        <v>0.16489999999999999</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.2863</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0.1946</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1.7286999999999999</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <v>2.68</v>
+      </c>
+      <c r="C34" s="8">
+        <v>1.7251000000000001</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <v>2.76</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1.7081999999999999</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
+        <v>2.85</v>
+      </c>
+      <c r="C36" s="8">
+        <v>1.6957</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <v>2.93</v>
+      </c>
+      <c r="C37" s="8">
+        <v>1.7188000000000001</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="17">
+        <v>3</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="18">
+        <v>0.1691</v>
+      </c>
+      <c r="E38" s="14">
+        <v>0.28510000000000002</v>
+      </c>
+      <c r="F38" s="18">
+        <v>0.19589999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F46F1A2-3464-46AB-AC0B-0CBD57F6E68E}">
-  <dimension ref="A2:J29"/>
+  <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="7" width="15.7109375" customWidth="1"/>
+    <col min="4" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="25">
         <v>0.10249999999999999</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="25">
         <v>0.1578</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="26">
         <v>0.1211</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="25">
         <v>0.15049999999999999</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="25">
         <v>0.24560000000000001</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="27">
         <v>0.17249999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="25">
         <v>0.14649999999999999</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="25">
         <v>0.24199999999999999</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="27">
         <v>0.16850000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="25">
         <v>0.13950000000000001</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="25">
         <v>0.23019999999999999</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="27">
         <v>0.16089999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="25"/>
+      <c r="H7" s="25">
+        <v>2.76E-2</v>
+      </c>
+      <c r="I7" s="25">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="J7" s="27">
+        <v>3.3799999999999997E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="25"/>
+      <c r="B8" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="25">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="I8" s="25">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="J8" s="27">
+        <v>3.1300000000000001E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="25"/>
+      <c r="A9" s="15"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="25"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-    </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-    </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Found a new dataset, continued training, added some notes, business as usual.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\gpu_tu_dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC05907-453A-4557-950F-51597294953A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785F77DE-869E-4E19-BA76-4BDFA358C849}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="165" windowWidth="21405" windowHeight="15435" activeTab="4" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="7395" yWindow="165" windowWidth="21405" windowHeight="15435" activeTab="1" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT_ML_ENG_MIX" sheetId="1" r:id="rId1"/>
     <sheet name="BERT_ML_DE_MIX" sheetId="5" r:id="rId2"/>
     <sheet name="BERT_DE_DE_MIX" sheetId="8" r:id="rId3"/>
     <sheet name="XLMR_ML_DE_MIX" sheetId="9" r:id="rId4"/>
-    <sheet name="GBERT_DE_DE_MIX" sheetId="11" r:id="rId5"/>
-    <sheet name="BERT_ML_DE_MIX_EXP" sheetId="10" r:id="rId6"/>
+    <sheet name="XLMR_DE_DE_MIX" sheetId="12" r:id="rId5"/>
+    <sheet name="GBERT_DE_DE_MIX" sheetId="11" r:id="rId6"/>
+    <sheet name="BERT_ML_DE_MIX_EXP" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="36">
   <si>
     <t>Language</t>
   </si>
@@ -75,9 +76,6 @@
   </si>
   <si>
     <t>German</t>
-  </si>
-  <si>
-    <t>Wikipedia/ ZEIT (3925/ 235)</t>
   </si>
   <si>
     <t>→</t>
@@ -160,6 +158,9 @@
   </si>
   <si>
     <t>DEEPSET/GBERT-BASE</t>
+  </si>
+  <si>
+    <t>WIKI/ NEWS/ MLSUM (3925/ 235)</t>
   </si>
 </sst>
 </file>
@@ -849,7 +850,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GBERT_DE_DE_MIX!$D$2</c:f>
+              <c:f>XLMR_DE_DE_MIX!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -870,14 +871,71 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-48EE-494A-9680-01B6A387DF8C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-48EE-494A-9680-01B6A387DF8C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>GBERT_DE_DE_MIX!$D$3:$D$10</c:f>
+              <c:f>(XLMR_DE_DE_MIX!$D$7,XLMR_DE_DE_MIX!$D$12,XLMR_DE_DE_MIX!$D$17,XLMR_DE_DE_MIX!$D$22,XLMR_DE_DE_MIX!$D$27,XLMR_DE_DE_MIX!$D$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.0499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.67E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6699999999999995E-2</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1147</c:v>
+                  <c:v>7.3400000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7400000000000005E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -885,7 +943,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-31E4-420A-A52A-0261E3DCEBBC}"/>
+              <c16:uniqueId val="{00000004-48EE-494A-9680-01B6A387DF8C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -894,7 +952,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>GBERT_DE_DE_MIX!$E$2</c:f>
+              <c:f>XLMR_DE_DE_MIX!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -915,14 +973,71 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-48EE-494A-9680-01B6A387DF8C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-48EE-494A-9680-01B6A387DF8C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>GBERT_DE_DE_MIX!$E$3:$E$10</c:f>
+              <c:f>(XLMR_DE_DE_MIX!$E$7,XLMR_DE_DE_MIX!$E$12,XLMR_DE_DE_MIX!$E$17,XLMR_DE_DE_MIX!$E$22,XLMR_DE_DE_MIX!$E$27,XLMR_DE_DE_MIX!$E$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.0599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9900000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8899999999999998E-2</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.21729999999999999</c:v>
+                  <c:v>8.5099999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10589999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -930,7 +1045,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-31E4-420A-A52A-0261E3DCEBBC}"/>
+              <c16:uniqueId val="{00000009-48EE-494A-9680-01B6A387DF8C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -939,7 +1054,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>GBERT_DE_DE_MIX!$F$2</c:f>
+              <c:f>XLMR_DE_DE_MIX!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -960,14 +1075,71 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-48EE-494A-9680-01B6A387DF8C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-48EE-494A-9680-01B6A387DF8C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>GBERT_DE_DE_MIX!$F$3:$F$10</c:f>
+              <c:f>(XLMR_DE_DE_MIX!$F$7,XLMR_DE_DE_MIX!$F$12,XLMR_DE_DE_MIX!$F$17,XLMR_DE_DE_MIX!$F$22,XLMR_DE_DE_MIX!$F$27,XLMR_DE_DE_MIX!$F$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.7799999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.24E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7299999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5600000000000006E-2</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1389</c:v>
+                  <c:v>7.1599999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7300000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -975,7 +1147,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-31E4-420A-A52A-0261E3DCEBBC}"/>
+              <c16:uniqueId val="{0000000E-48EE-494A-9680-01B6A387DF8C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -998,6 +1170,744 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533794816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="533794816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533795144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GBERT_DE_DE_MIX!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="21835E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>GBERT_DE_DE_MIX!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.9932999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5619000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1392000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8950999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7063000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5735000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4460999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2F0F-4A9D-9145-0FAFF4B4EDC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="530566160"/>
+        <c:axId val="530567800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="530566160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530567800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="530567800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530566160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" b="1">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Scores</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GBERT_DE_DE_MIX!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Precision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="21835E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(GBERT_DE_DE_MIX!$D$7,GBERT_DE_DE_MIX!$D$12,GBERT_DE_DE_MIX!$D$17,GBERT_DE_DE_MIX!$D$27,GBERT_DE_DE_MIX!$D$32)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1147</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15490000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16489999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-31E4-420A-A52A-0261E3DCEBBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GBERT_DE_DE_MIX!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="325D72"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(GBERT_DE_DE_MIX!$E$7,GBERT_DE_DE_MIX!$E$12,GBERT_DE_DE_MIX!$E$17,GBERT_DE_DE_MIX!$E$27,GBERT_DE_DE_MIX!$E$32)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.21729999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27410000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2863</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-31E4-420A-A52A-0261E3DCEBBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GBERT_DE_DE_MIX!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-Measure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="A74343"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(GBERT_DE_DE_MIX!$F$7,GBERT_DE_DE_MIX!$F$12,GBERT_DE_DE_MIX!$F$17,GBERT_DE_DE_MIX!$F$27,GBERT_DE_DE_MIX!$F$32)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1389</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1709</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1946</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-31E4-420A-A52A-0261E3DCEBBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="533795144"/>
+        <c:axId val="533794816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="533795144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1914,28 +2824,28 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.3719999999999999</c:v>
+                  <c:v>5.1638000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7545999999999999</c:v>
+                  <c:v>4.0023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4763999999999999</c:v>
+                  <c:v>3.7578999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2736999999999998</c:v>
+                  <c:v>3.5360999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2080000000000002</c:v>
+                  <c:v>3.38611</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0129999999999999</c:v>
+                  <c:v>3.2854999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9557</c:v>
+                  <c:v>3.1818</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9168000000000001</c:v>
+                  <c:v>3.0933999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,29 +3138,8 @@
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>7.2599999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1149</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.13120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.13880000000000001</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14680000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.15129999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.15509999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.15579999999999999</c:v>
+                  <c:v>5.2900000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2294,29 +3183,8 @@
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.1545</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2278</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25290000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.27010000000000001</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27889999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.28639999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.28970000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.29149999999999998</c:v>
+                  <c:v>9.6500000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2360,29 +3228,8 @@
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>9.1800000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.14169999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.16109999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.17080000000000001</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1792</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1845</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.1885</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.1893</c:v>
+                  <c:v>6.3899999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4356,7 +5203,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GBERT_DE_DE_MIX!$C$2</c:f>
+              <c:f>XLMR_DE_DE_MIX!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4379,33 +5226,114 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GBERT_DE_DE_MIX!$C$3:$C$10</c:f>
+              <c:f>XLMR_DE_DE_MIX!$C$3:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>4.9932999999999996</c:v>
+                  <c:v>9.2078000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5619000000000001</c:v>
+                  <c:v>7.0819000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1392000000000002</c:v>
+                  <c:v>6.8507999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8950999999999998</c:v>
+                  <c:v>6.7034000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7063000000000001</c:v>
+                  <c:v>6.5815000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5735000000000001</c:v>
+                  <c:v>6.4364999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4630000000000001</c:v>
+                  <c:v>6.3384</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4460999999999999</c:v>
+                  <c:v>6.2687999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.2225999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.1776999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.1134000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0879000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.0160999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.0015999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.9497999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9566999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.9414999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.9051</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.8924000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.8311999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.8193999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.7632000000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.7611999999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.7385999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.6669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.6505999999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.6169000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.6081000000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.5918000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.6079999999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.5968</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.5982000000000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.4985999999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.4311999999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.4130000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4413,7 +5341,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2F0F-4A9D-9145-0FAFF4B4EDC6}"/>
+              <c16:uniqueId val="{00000000-B8C7-4053-8948-290B1B9F6A80}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4628,6 +5556,86 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6006,6 +7014,1025 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -10424,6 +12451,87 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03C531BD-034B-4480-A84D-3AFE8C9D5715}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEB28A26-02D0-4FF4-AC5B-85E070A91D04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{894DCD04-5085-4646-94DA-95ED03FBE1BE}"/>
             </a:ext>
           </a:extLst>
@@ -10860,7 +12968,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -10884,7 +12992,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -10905,7 +13013,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>10</v>
@@ -10929,7 +13037,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>10</v>
@@ -11315,13 +13423,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="17">
         <v>3</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="14">
         <v>0.10249999999999999</v>
@@ -11386,9 +13494,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB4DBC8-2BC1-41BA-920C-B3169F829E6E}">
-  <dimension ref="A2:I34"/>
+  <dimension ref="A2:I40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -11399,7 +13507,7 @@
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -11420,22 +13528,16 @@
       </c>
       <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
-        <v>0.36</v>
+        <v>0.05</v>
       </c>
       <c r="C3" s="7">
-        <v>3.3719999999999999</v>
-      </c>
-      <c r="D3" s="7">
-        <v>7.2599999999999998E-2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.1545</v>
-      </c>
-      <c r="F3" s="9">
-        <v>9.1800000000000007E-2</v>
-      </c>
+        <v>5.1638000000000002</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="9"/>
       <c r="H3" s="11" t="s">
         <v>0</v>
       </c>
@@ -11443,320 +13545,400 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
-        <v>0.71</v>
+        <v>0.11</v>
       </c>
       <c r="C4" s="8">
-        <v>2.7545999999999999</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0.1149</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.2278</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0.14169999999999999</v>
-      </c>
+        <v>4.0023</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="1"/>
       <c r="H4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
-        <v>1.07</v>
+        <v>0.16</v>
       </c>
       <c r="C5" s="8">
-        <v>2.4763999999999999</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.13120000000000001</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.25290000000000001</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0.16109999999999999</v>
-      </c>
+        <v>3.7578999999999998</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="1"/>
       <c r="H5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
-        <v>1.42</v>
+        <v>0.21</v>
       </c>
       <c r="C6" s="8">
-        <v>2.2736999999999998</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0.13880000000000001</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.27010000000000001</v>
-      </c>
-      <c r="F6" s="10">
-        <v>0.17080000000000001</v>
-      </c>
+        <v>3.5360999999999998</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
-        <v>1.78</v>
+        <v>0.27</v>
       </c>
       <c r="C7" s="8">
-        <v>2.2080000000000002</v>
+        <v>3.38611</v>
       </c>
       <c r="D7" s="8">
-        <v>0.14680000000000001</v>
+        <v>5.2900000000000003E-2</v>
       </c>
       <c r="E7" s="3">
-        <v>0.27889999999999998</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="F7" s="10">
-        <v>0.1792</v>
+        <v>6.3899999999999998E-2</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3.2854999999999999</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>0.37</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3.1818</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3.0933999999999999</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3.0148999999999999</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2.9405999999999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.13239999999999999</v>
+      </c>
+      <c r="F12" s="10">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2.8774000000000002</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>0.64</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2.8239999999999998</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2.7881</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C16" s="8">
+        <v>2.7515999999999998</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2.7159</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="6"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="6"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="6"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="6"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="6"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="6"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="17">
+        <v>3</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <v>2.13</v>
-      </c>
-      <c r="C8" s="8">
-        <v>2.0129999999999999</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0.15129999999999999</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.28639999999999999</v>
-      </c>
-      <c r="F8" s="10">
-        <v>0.1845</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="C9" s="8">
-        <v>1.9557</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.15509999999999999</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.28970000000000001</v>
-      </c>
-      <c r="F9" s="10">
-        <v>0.1885</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <v>2.85</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1.9168000000000001</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.15579999999999999</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.29149999999999998</v>
-      </c>
-      <c r="F10" s="10">
-        <v>0.1893</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="17">
-        <v>3</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="D40" s="14">
         <v>0.15049999999999999</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E40" s="14">
         <v>0.24560000000000001</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F40" s="14">
         <v>0.17249999999999999</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11773,7 +13955,7 @@
   <dimension ref="A2:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11848,7 +14030,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -11872,7 +14054,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -11893,10 +14075,10 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -11917,10 +14099,10 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -11979,13 +14161,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="17">
         <v>3</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="18">
         <v>0.14649999999999999</v>
@@ -12142,7 +14324,7 @@
   <dimension ref="A2:I40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12205,7 +14387,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -12223,7 +14405,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -12238,10 +14420,10 @@
       <c r="F6" s="10"/>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -12262,10 +14444,10 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -12688,13 +14870,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B40" s="17">
         <v>3</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="18">
         <v>0.13950000000000001</v>
@@ -12717,11 +14899,560 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B554BE-C186-4BDD-933B-F8710D86BA47}">
+  <dimension ref="A2:I38"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="C3" s="7">
+        <v>9.2078000000000007</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="9"/>
+      <c r="H3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="C4" s="8">
+        <v>7.0819000000000001</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="8">
+        <v>6.8507999999999996</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="C6" s="8">
+        <v>6.7034000000000002</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6.5815000000000001</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2.7799999999999998E-2</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="8">
+        <v>6.4364999999999997</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="C9" s="8">
+        <v>6.3384</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6.2687999999999997</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="8">
+        <v>6.2225999999999999</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>0.84</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6.1776999999999997</v>
+      </c>
+      <c r="D12" s="8">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="F12" s="10">
+        <v>4.24E-2</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="C13" s="8">
+        <v>6.1134000000000004</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>6.0879000000000003</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C15" s="8">
+        <v>6.0160999999999998</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>1.17</v>
+      </c>
+      <c r="C16" s="8">
+        <v>6.0015999999999998</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>1.26</v>
+      </c>
+      <c r="C17" s="8">
+        <v>5.9497999999999998</v>
+      </c>
+      <c r="D17" s="8">
+        <v>5.67E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>6.9900000000000004E-2</v>
+      </c>
+      <c r="F17" s="10">
+        <v>5.7299999999999997E-2</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>1.34</v>
+      </c>
+      <c r="C18" s="8">
+        <v>5.9566999999999997</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>1.42</v>
+      </c>
+      <c r="C19" s="8">
+        <v>5.9414999999999996</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>1.51</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5.9051</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>1.59</v>
+      </c>
+      <c r="C21" s="8">
+        <v>5.8924000000000003</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>1.67</v>
+      </c>
+      <c r="C22" s="8">
+        <v>5.8311999999999999</v>
+      </c>
+      <c r="D22" s="8">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="F22" s="10">
+        <v>6.5600000000000006E-2</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>1.76</v>
+      </c>
+      <c r="C23" s="8">
+        <v>5.8193999999999999</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>1.84</v>
+      </c>
+      <c r="C24" s="8">
+        <v>5.7632000000000003</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>1.93</v>
+      </c>
+      <c r="C25" s="8">
+        <v>5.7611999999999997</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C26" s="8">
+        <v>5.7385999999999999</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>2.09</v>
+      </c>
+      <c r="C27" s="8">
+        <v>5.6669999999999998</v>
+      </c>
+      <c r="D27" s="8">
+        <v>7.3400000000000007E-2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="F27" s="10">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="C28" s="8">
+        <v>5.6505999999999998</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C29" s="8">
+        <v>5.6169000000000002</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <v>2.34</v>
+      </c>
+      <c r="C30" s="8">
+        <v>5.6081000000000003</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="C31" s="8">
+        <v>5.5918000000000001</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="6">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="C32" s="8">
+        <v>5.6079999999999997</v>
+      </c>
+      <c r="D32" s="8">
+        <v>8.7400000000000005E-2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.10589999999999999</v>
+      </c>
+      <c r="F32" s="10">
+        <v>8.7300000000000003E-2</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="C33" s="8">
+        <v>5.5968</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <v>2.68</v>
+      </c>
+      <c r="C34" s="8">
+        <v>5.5982000000000003</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <v>2.76</v>
+      </c>
+      <c r="C35" s="8">
+        <v>5.4985999999999997</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="6">
+        <v>2.85</v>
+      </c>
+      <c r="C36" s="8">
+        <v>5.4311999999999996</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <v>2.93</v>
+      </c>
+      <c r="C37" s="8">
+        <v>5.4130000000000003</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="17">
+        <v>3</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="18">
+        <v>7.7700000000000005E-2</v>
+      </c>
+      <c r="E38" s="14">
+        <v>0.1009</v>
+      </c>
+      <c r="F38" s="18">
+        <v>7.9899999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AF756F-671F-47D9-8966-F6A5F7632BF1}">
   <dimension ref="A2:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12784,7 +15515,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -12802,7 +15533,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -12817,10 +15548,10 @@
       <c r="F6" s="10"/>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -12841,10 +15572,10 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -13236,13 +15967,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" s="17">
         <v>3</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" s="18">
         <v>0.1691</v>
@@ -13264,7 +15995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F46F1A2-3464-46AB-AC0B-0CBD57F6E68E}">
   <dimension ref="A2:J27"/>
   <sheetViews>
@@ -13280,51 +16011,51 @@
   <sheetData>
     <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>33</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>21</v>
-      </c>
       <c r="E3" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="25">
         <v>0.10249999999999999</v>
@@ -13338,22 +16069,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="25">
         <v>0.15049999999999999</v>
@@ -13367,22 +16098,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="25">
         <v>0.14649999999999999</v>
@@ -13396,22 +16127,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="25">
         <v>0.13950000000000001</v>
@@ -13425,22 +16156,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>23</v>
-      </c>
       <c r="E7" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="25">
         <v>2.76E-2</v>
@@ -13454,22 +16185,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>23</v>
-      </c>
       <c r="F8" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="25">
         <v>2.5899999999999999E-2</v>

</xml_diff>

<commit_message>
Updated both main chapters.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\gpu_tu_dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C9DD25-E3DE-4522-97F7-CDF8A550ACC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D150F95D-FA46-48FE-992B-628A174171E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="7395" yWindow="165" windowWidth="21405" windowHeight="15435" activeTab="2" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT_EN" sheetId="1" r:id="rId1"/>
     <sheet name="BERT_DE" sheetId="5" r:id="rId2"/>
-    <sheet name="BERT_ML" sheetId="14" r:id="rId3"/>
-    <sheet name="GBERT_DE" sheetId="11" r:id="rId4"/>
+    <sheet name="GBERT_DE" sheetId="11" r:id="rId3"/>
+    <sheet name="BERT_ML" sheetId="14" r:id="rId4"/>
     <sheet name="XLMR_DE" sheetId="9" r:id="rId5"/>
     <sheet name="BART_DE" sheetId="13" r:id="rId6"/>
   </sheets>
@@ -3859,7 +3859,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT_ML!$C$2</c:f>
+              <c:f>GBERT_DE!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3878,33 +3878,66 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="21835E"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="21835E"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>BERT_ML!$C$3:$C$57</c:f>
+              <c:f>GBERT_DE!$C$3:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>5.2130999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9064999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6002000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3980999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2467999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1349</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0236999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9401999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8662000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8081</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7570999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.7241</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6924000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6613000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6387</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3503-461B-A612-97155D083CCF}"/>
+              <c16:uniqueId val="{00000000-2F0F-4A9D-9145-0FAFF4B4EDC6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3916,7 +3949,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="530566160"/>
         <c:axId val="530567800"/>
@@ -4162,7 +4194,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT_ML!$D$2</c:f>
+              <c:f>GBERT_DE!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4185,17 +4217,23 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(BERT_ML!$D$7,BERT_ML!$D$12,BERT_ML!$D$17,BERT_ML!$D$22,BERT_ML!$D$27,BERT_ML!$D$32,BERT_ML!$D$37,BERT_ML!$D$42,BERT_ML!$D$47,BERT_ML!$D$52,BERT_ML!$D$57)</c:f>
+              <c:f>(GBERT_DE!$D$7,GBERT_DE!$D$12,GBERT_DE!$D$17,GBERT_DE!$D$27,GBERT_DE!$D$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.7799999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4599999999999995E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2755-4B6C-8AEE-66BF0BD83FA4}"/>
+              <c16:uniqueId val="{00000000-31E4-420A-A52A-0261E3DCEBBC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4204,7 +4242,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT_ML!$E$2</c:f>
+              <c:f>GBERT_DE!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4227,17 +4265,23 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(BERT_ML!$E$7,BERT_ML!$E$12,BERT_ML!$E$17,BERT_ML!$E$22,BERT_ML!$E$27,BERT_ML!$E$32,BERT_ML!$E$37,BERT_ML!$E$42,BERT_ML!$E$47,BERT_ML!$E$52,BERT_ML!$E$57)</c:f>
+              <c:f>(GBERT_DE!$E$7,GBERT_DE!$E$12,GBERT_DE!$E$17,GBERT_DE!$E$27,GBERT_DE!$E$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1086</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1502</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2755-4B6C-8AEE-66BF0BD83FA4}"/>
+              <c16:uniqueId val="{00000004-31E4-420A-A52A-0261E3DCEBBC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4246,7 +4290,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>BERT_ML!$F$2</c:f>
+              <c:f>GBERT_DE!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4269,17 +4313,23 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(BERT_ML!$F$7,BERT_ML!$F$12,BERT_ML!$F$17,BERT_ML!$F$22,BERT_ML!$F$27,BERT_ML!$F$32,BERT_ML!$F$37,BERT_ML!$F$42,BERT_ML!$F$47,BERT_ML!$F$52,BERT_ML!$F$57)</c:f>
+              <c:f>(GBERT_DE!$F$7,GBERT_DE!$F$12,GBERT_DE!$F$17,GBERT_DE!$F$27,GBERT_DE!$F$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.0900000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1023</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2755-4B6C-8AEE-66BF0BD83FA4}"/>
+              <c16:uniqueId val="{00000005-31E4-420A-A52A-0261E3DCEBBC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4540,7 +4590,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GBERT_DE!$C$2</c:f>
+              <c:f>BERT_ML!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4559,21 +4609,33 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="21835E"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="21835E"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GBERT_DE!$C$3:$C$10</c:f>
+              <c:f>BERT_ML!$C$3:$C$57</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="55"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2F0F-4A9D-9145-0FAFF4B4EDC6}"/>
+              <c16:uniqueId val="{00000000-3503-461B-A612-97155D083CCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4585,6 +4647,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="530566160"/>
         <c:axId val="530567800"/>
@@ -4830,7 +4893,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GBERT_DE!$D$2</c:f>
+              <c:f>BERT_ML!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4853,17 +4916,17 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(GBERT_DE!$D$7,GBERT_DE!$D$12,GBERT_DE!$D$17,GBERT_DE!$D$27,GBERT_DE!$D$32)</c:f>
+              <c:f>(BERT_ML!$D$7,BERT_ML!$D$12,BERT_ML!$D$17,BERT_ML!$D$22,BERT_ML!$D$27,BERT_ML!$D$32,BERT_ML!$D$37,BERT_ML!$D$42,BERT_ML!$D$47,BERT_ML!$D$52,BERT_ML!$D$57)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="11"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-31E4-420A-A52A-0261E3DCEBBC}"/>
+              <c16:uniqueId val="{00000000-2755-4B6C-8AEE-66BF0BD83FA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4872,7 +4935,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>GBERT_DE!$E$2</c:f>
+              <c:f>BERT_ML!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4895,17 +4958,17 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(GBERT_DE!$E$7,GBERT_DE!$E$12,GBERT_DE!$E$17,GBERT_DE!$E$27,GBERT_DE!$E$32)</c:f>
+              <c:f>(BERT_ML!$E$7,BERT_ML!$E$12,BERT_ML!$E$17,BERT_ML!$E$22,BERT_ML!$E$27,BERT_ML!$E$32,BERT_ML!$E$37,BERT_ML!$E$42,BERT_ML!$E$47,BERT_ML!$E$52,BERT_ML!$E$57)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="11"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-31E4-420A-A52A-0261E3DCEBBC}"/>
+              <c16:uniqueId val="{00000001-2755-4B6C-8AEE-66BF0BD83FA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4914,7 +4977,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>GBERT_DE!$F$2</c:f>
+              <c:f>BERT_ML!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4937,17 +5000,17 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(GBERT_DE!$F$7,GBERT_DE!$F$12,GBERT_DE!$F$17,GBERT_DE!$F$27,GBERT_DE!$F$32)</c:f>
+              <c:f>(BERT_ML!$F$7,BERT_ML!$F$12,BERT_ML!$F$17,BERT_ML!$F$22,BERT_ML!$F$27,BERT_ML!$F$32,BERT_ML!$F$37,BERT_ML!$F$42,BERT_ML!$F$47,BERT_ML!$F$52,BERT_ML!$F$57)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="11"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-31E4-420A-A52A-0261E3DCEBBC}"/>
+              <c16:uniqueId val="{00000002-2755-4B6C-8AEE-66BF0BD83FA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12300,7 +12363,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58D00992-93D8-4370-AFCC-1C5C0707C29C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{894DCD04-5085-4646-94DA-95ED03FBE1BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12338,7 +12401,7 @@
         <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{790B1CAC-4684-4795-A8F1-71C763899E8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E85E22-6818-4926-91BF-60564AB9F24A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12381,7 +12444,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{894DCD04-5085-4646-94DA-95ED03FBE1BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58D00992-93D8-4370-AFCC-1C5C0707C29C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12419,7 +12482,7 @@
         <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E85E22-6818-4926-91BF-60564AB9F24A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{790B1CAC-4684-4795-A8F1-71C763899E8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13507,8 +13570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB4DBC8-2BC1-41BA-920C-B3169F829E6E}">
   <dimension ref="A2:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14282,13 +14345,13 @@
         <v>15</v>
       </c>
       <c r="D58" s="14">
-        <v>0.15049999999999999</v>
+        <v>0.1052</v>
       </c>
       <c r="E58" s="14">
-        <v>0.24560000000000001</v>
+        <v>0.1593</v>
       </c>
       <c r="F58" s="14">
-        <v>0.17249999999999999</v>
+        <v>0.1197</v>
       </c>
     </row>
   </sheetData>
@@ -14302,6 +14365,450 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AF756F-671F-47D9-8966-F6A5F7632BF1}">
+  <dimension ref="A2:I38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="7">
+        <v>5.2130999999999998</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="9"/>
+      <c r="H3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.9064999999999999</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3.6002000000000001</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3.3980999999999999</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>0.27</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3.2467999999999999</v>
+      </c>
+      <c r="D7" s="8">
+        <v>5.7799999999999997E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.1086</v>
+      </c>
+      <c r="F7" s="10">
+        <v>7.0900000000000005E-2</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3.1349</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>0.37</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3.0236999999999998</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2.9401999999999999</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2.8662000000000001</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2.8081</v>
+      </c>
+      <c r="D12" s="8">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.1502</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.1023</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2.7570999999999999</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>0.64</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2.7241</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2.6924000000000001</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C16" s="8">
+        <v>2.6613000000000002</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2.6387</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="6"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="6"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="6"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="6"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="17">
+        <v>3</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="18">
+        <v>0.1691</v>
+      </c>
+      <c r="E38" s="14">
+        <v>0.28510000000000002</v>
+      </c>
+      <c r="F38" s="18">
+        <v>0.19589999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C848A1E6-F364-4342-9FA6-BDF6C94FACDC}">
   <dimension ref="A2:I58"/>
   <sheetViews>
@@ -14801,378 +15308,6 @@
       </c>
       <c r="F58" s="14">
         <v>0.17249999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H2:I2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AF756F-671F-47D9-8966-F6A5F7632BF1}">
-  <dimension ref="A2:I38"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="9"/>
-      <c r="H3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="6"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="6"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="17">
-        <v>3</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="18">
-        <v>0.1691</v>
-      </c>
-      <c r="E38" s="14">
-        <v>0.28510000000000002</v>
-      </c>
-      <c r="F38" s="18">
-        <v>0.19589999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote a lot of structural text.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/gpu_tu_dresden/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\gpu_tu_dresden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E78193-5E93-4A6E-9AB6-04B182012FDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17CAF40-FDC2-45BA-9726-0D71475AE8B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="165" windowWidth="21405" windowHeight="15435" activeTab="5" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="7395" yWindow="165" windowWidth="21405" windowHeight="15435" firstSheet="3" activeTab="6" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT_EN" sheetId="1" r:id="rId1"/>
@@ -290,9 +290,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF21835E"/>
+      <color rgb="FFA74343"/>
       <color rgb="FF325D72"/>
-      <color rgb="FFA74343"/>
-      <color rgb="FF21835E"/>
     </mruColors>
   </colors>
   <extLst>
@@ -792,7 +792,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dPt>
-            <c:idx val="1"/>
+            <c:idx val="0"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -800,20 +800,15 @@
             <c:spPr>
               <a:ln w="28575" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="21835E"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="5"/>
+            <c:idx val="2"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -821,24 +816,28 @@
             <c:spPr>
               <a:ln w="28575" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="21835E"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR_EN!$D$7,XLMR_EN!$D$12,XLMR_EN!$D$17,XLMR_EN!$D$22,XLMR_EN!$D$27,XLMR_EN!$D$32,XLMR_EN!$D$37)</c:f>
+              <c:f>(XLMR_EN!$D$12,XLMR_EN!$D$22,XLMR_EN!$D$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.01E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4100000000000003E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -876,7 +875,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dPt>
-            <c:idx val="1"/>
+            <c:idx val="0"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -884,20 +883,15 @@
             <c:spPr>
               <a:ln w="28575" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:srgbClr val="325D72"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="5"/>
+            <c:idx val="2"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -905,31 +899,35 @@
             <c:spPr>
               <a:ln w="28575" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:srgbClr val="325D72"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR_EN!$E$7,XLMR_EN!$E$12,XLMR_EN!$E$17,XLMR_EN!$E$22,XLMR_EN!$E$27,XLMR_EN!$E$32,XLMR_EN!$E$37)</c:f>
+              <c:f>(XLMR_EN!$E$12,XLMR_EN!$E$22,XLMR_EN!$E$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.2699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.3700000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12470000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
+              <c16:uniqueId val="{00000010-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -960,7 +958,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dPt>
-            <c:idx val="1"/>
+            <c:idx val="0"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -968,20 +966,15 @@
             <c:spPr>
               <a:ln w="28575" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:srgbClr val="A74343"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="5"/>
+            <c:idx val="2"/>
             <c:marker>
               <c:symbol val="none"/>
             </c:marker>
@@ -989,31 +982,35 @@
             <c:spPr>
               <a:ln w="28575" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:srgbClr val="A74343"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>(XLMR_EN!$F$7,XLMR_EN!$F$12,XLMR_EN!$F$17,XLMR_EN!$F$22,XLMR_EN!$F$27,XLMR_EN!$F$32,XLMR_EN!$F$37)</c:f>
+              <c:f>(XLMR_EN!$F$12,XLMR_EN!$F$22,XLMR_EN!$F$32)</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0199999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1045</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
+              <c16:uniqueId val="{00000011-9BAA-45FA-8F2F-8E21EBD3A7DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2292,6 +2289,72 @@
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>7.5473999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9588000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8418999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7567000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6959999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6492000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6054000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5720999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5484999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5247000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.4981999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.4927000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.4714999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.4587000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.4337</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.4264999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.4154999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4047000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.3935000000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.3757999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.3661000000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.3712</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2624,6 +2687,12 @@
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>1.04E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3100000000000001E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2708,6 +2777,12 @@
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>4.8999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2792,6 +2867,12 @@
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>6.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0999999999999996E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7541,10 +7622,100 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>XLMR_EN!$C$3:$C$39</c:f>
+              <c:f>XLMR_EN!$C$3:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>7.2043999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7281000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6013999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5136000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4484000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3666999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1420000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0591999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9679000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9344999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7065000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3951000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.1993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0330000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.8780999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5864000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.4721000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.3590999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.2767999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.1623000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.0658000000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.0030999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.9096000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8479999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.7913000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.7522000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.7301000000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.7054</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.6688999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -20574,6 +20745,485 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8D7B0E-2744-461D-949E-D223AB56EB6D}">
+  <dimension ref="A2:I34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>7.2043999999999997</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="9"/>
+      <c r="H3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>6.7281000000000004</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>6.6013999999999999</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>6.5136000000000003</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6.4484000000000004</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="C8" s="8">
+        <v>6.3666999999999998</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="C9" s="8">
+        <v>6.1420000000000003</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6.0591999999999997</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5.9679000000000002</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5.9344999999999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1.01E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C13" s="8">
+        <v>5.7065000000000001</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>1.19</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5.3951000000000002</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>1.29</v>
+      </c>
+      <c r="C15" s="8">
+        <v>5.1993</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>1.38</v>
+      </c>
+      <c r="C16" s="8">
+        <v>5.0330000000000004</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>1.48</v>
+      </c>
+      <c r="C17" s="8">
+        <v>4.8780999999999999</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>1.58</v>
+      </c>
+      <c r="C18" s="8">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>1.68</v>
+      </c>
+      <c r="C19" s="8">
+        <v>4.5864000000000003</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>1.78</v>
+      </c>
+      <c r="C20" s="8">
+        <v>4.4721000000000002</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>1.88</v>
+      </c>
+      <c r="C21" s="8">
+        <v>4.3590999999999998</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>1.98</v>
+      </c>
+      <c r="C22" s="8">
+        <v>4.2767999999999997</v>
+      </c>
+      <c r="D22" s="8">
+        <v>7.3599999999999999E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>9.3700000000000006E-2</v>
+      </c>
+      <c r="F22" s="10">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>2.08</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4.1623000000000001</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>2.17</v>
+      </c>
+      <c r="C24" s="8">
+        <v>4.0658000000000003</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>2.27</v>
+      </c>
+      <c r="C25" s="8">
+        <v>4.0030999999999999</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>2.37</v>
+      </c>
+      <c r="C26" s="8">
+        <v>3.9096000000000002</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="C27" s="8">
+        <v>3.8479999999999999</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>2.57</v>
+      </c>
+      <c r="C28" s="8">
+        <v>3.7913000000000001</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>2.67</v>
+      </c>
+      <c r="C29" s="8">
+        <v>3.7522000000000002</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <v>2.77</v>
+      </c>
+      <c r="C30" s="8">
+        <v>3.7301000000000002</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>2.87</v>
+      </c>
+      <c r="C31" s="8">
+        <v>3.7054</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="6">
+        <v>2.97</v>
+      </c>
+      <c r="C32" s="8">
+        <v>3.6688999999999998</v>
+      </c>
+      <c r="D32" s="8">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.12470000000000001</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0.1045</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="17">
+        <v>3</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="14">
+        <v>8.8800000000000004E-2</v>
+      </c>
+      <c r="E33" s="14">
+        <v>0.1176</v>
+      </c>
+      <c r="F33" s="14">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42CEBC-4DF1-4EAE-9662-1F6C023E63EA}">
   <dimension ref="A2:I59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -20588,528 +21238,6 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="9"/>
-      <c r="H3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="6"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="6"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="10"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="6"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="10"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="6"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="10"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="6"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="10"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="6"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="10"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="6"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="10"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="6"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="10"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="6"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="10"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="6"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="10"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="6"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="10"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="6"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="10"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="6"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="10"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="6"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="10"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="6"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="10"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="6"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="10"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="6"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="10"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="6"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="10"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="6"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="10"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="6"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="10"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="6"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="10"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="6"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="10"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B59" s="17">
-        <v>3</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="14">
-        <v>0</v>
-      </c>
-      <c r="E59" s="14">
-        <v>0</v>
-      </c>
-      <c r="F59" s="14">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H2:I2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42CEBC-4DF1-4EAE-9662-1F6C023E63EA}">
-  <dimension ref="A2:I59"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
@@ -21874,8 +22002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCCAA2A-009C-4C5D-A2B1-28765BD19D0C}">
   <dimension ref="A2:I59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21907,8 +22035,12 @@
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="C3" s="7">
+        <v>7.5473999999999997</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="3"/>
       <c r="F3" s="9"/>
@@ -21920,8 +22052,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>6.9588000000000001</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="3"/>
       <c r="F4" s="10"/>
@@ -21934,8 +22070,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="C5" s="8">
+        <v>6.8418999999999999</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="3"/>
       <c r="F5" s="10"/>
@@ -21948,8 +22088,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C6" s="8">
+        <v>6.7567000000000004</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="3"/>
       <c r="F6" s="10"/>
@@ -21962,8 +22106,12 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6.6959999999999997</v>
+      </c>
       <c r="D7" s="8"/>
       <c r="E7" s="3"/>
       <c r="F7" s="10"/>
@@ -21976,24 +22124,36 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="C8" s="8">
+        <v>6.6492000000000004</v>
+      </c>
       <c r="D8" s="8"/>
       <c r="E8" s="3"/>
       <c r="F8" s="10"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="8">
+        <v>6.6054000000000004</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="3"/>
       <c r="F9" s="10"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6.5720999999999998</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="3"/>
       <c r="F10" s="10"/>
@@ -22001,112 +22161,180 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="C11" s="8">
+        <v>6.5484999999999998</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="3"/>
       <c r="F11" s="10"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="10"/>
+      <c r="B12" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6.5247000000000002</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1.04E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="F12" s="10">
+        <v>6.3E-3</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="C13" s="8">
+        <v>6.4981999999999998</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="3"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="C14" s="8">
+        <v>6.4927000000000001</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="3"/>
       <c r="F14" s="10"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="C15" s="8">
+        <v>6.4714999999999998</v>
+      </c>
       <c r="D15" s="8"/>
       <c r="E15" s="3"/>
       <c r="F15" s="10"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="8">
+        <v>6.4587000000000003</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="3"/>
       <c r="F16" s="10"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="6">
+        <v>0.54</v>
+      </c>
+      <c r="C17" s="8">
+        <v>6.4337</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="3"/>
       <c r="F17" s="10"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="6">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C18" s="8">
+        <v>6.4264999999999999</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="3"/>
       <c r="F18" s="10"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="6">
+        <v>0.61</v>
+      </c>
+      <c r="C19" s="8">
+        <v>6.4154999999999998</v>
+      </c>
       <c r="D19" s="8"/>
       <c r="E19" s="3"/>
       <c r="F19" s="10"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="C20" s="8">
+        <v>6.4047000000000001</v>
+      </c>
       <c r="D20" s="8"/>
       <c r="E20" s="3"/>
       <c r="F20" s="10"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="8"/>
+      <c r="B21" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="C21" s="8">
+        <v>6.3935000000000004</v>
+      </c>
       <c r="D21" s="8"/>
       <c r="E21" s="3"/>
       <c r="F21" s="10"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="10"/>
+      <c r="B22" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="C22" s="8">
+        <v>6.3757999999999999</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>6.3E-3</v>
+      </c>
+      <c r="F22" s="10">
+        <v>8.0999999999999996E-3</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="8"/>
+      <c r="B23" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C23" s="8">
+        <v>6.3661000000000003</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="3"/>
       <c r="F23" s="10"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="8"/>
+      <c r="B24" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="C24" s="8">
+        <v>6.3712</v>
+      </c>
       <c r="D24" s="8"/>
       <c r="E24" s="3"/>
       <c r="F24" s="10"/>

</xml_diff>